<commit_message>
Student and Questions Export
</commit_message>
<xml_diff>
--- a/public/file/Studentlist.xlsx
+++ b/public/file/Studentlist.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -43,73 +43,10 @@
     <t>Patty O'Furniture.</t>
   </si>
   <si>
-    <t>Paddy O'Furniture.</t>
-  </si>
-  <si>
-    <t>Olive Yew.</t>
-  </si>
-  <si>
-    <t>Aida Bugg.</t>
-  </si>
-  <si>
-    <t>Maureen Biologist.</t>
-  </si>
-  <si>
-    <t>Teri Dactyl.</t>
-  </si>
-  <si>
-    <t>Peg Legge.</t>
-  </si>
-  <si>
-    <t>Allie Grater.</t>
-  </si>
-  <si>
     <t>202-555-0111</t>
   </si>
   <si>
-    <t>202-555-0188</t>
-  </si>
-  <si>
-    <t>202-555-0129</t>
-  </si>
-  <si>
-    <t>202-555-0141</t>
-  </si>
-  <si>
-    <t>202-555-0116</t>
-  </si>
-  <si>
-    <t>202-555-0177</t>
-  </si>
-  <si>
-    <t>202-555-0603</t>
-  </si>
-  <si>
-    <t>202-555-0139</t>
-  </si>
-  <si>
     <t>uraeus@icloud.com</t>
-  </si>
-  <si>
-    <t>fairbank@outlook.com</t>
-  </si>
-  <si>
-    <t>afeldspar@msn.com</t>
-  </si>
-  <si>
-    <t>redingtn@me.com</t>
-  </si>
-  <si>
-    <t>sokol@att.net</t>
-  </si>
-  <si>
-    <t>tezbo@live.com</t>
-  </si>
-  <si>
-    <t>tokuhirom@aol.com</t>
-  </si>
-  <si>
-    <t>inico@icloud.com</t>
   </si>
   <si>
     <t>btech</t>
@@ -456,7 +393,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -501,205 +438,44 @@
         <v>3568981</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="H2">
         <v>12345678</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>1245871</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>12345678</v>
-      </c>
+      <c r="A3" s="1"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>2145871</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4">
-        <v>12345678</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>3256891</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5">
-        <v>12345678</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6">
-        <v>3256591</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6">
-        <v>12345678</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>1234561</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7">
-        <v>12345678</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>49198531</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8">
-        <v>12345678</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9">
-        <v>49198521</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9">
-        <v>12345678</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>

<commit_message>
Quiz start button create
</commit_message>
<xml_diff>
--- a/public/file/Studentlist.xlsx
+++ b/public/file/Studentlist.xlsx
@@ -2,19 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" forceFullCalc="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -34,28 +36,10 @@
     <t>mobile</t>
   </si>
   <si>
-    <t xml:space="preserve">email </t>
+    <t>email</t>
   </si>
   <si>
     <t>password</t>
-  </si>
-  <si>
-    <t>Patty O'Furniture.</t>
-  </si>
-  <si>
-    <t>202-555-0111</t>
-  </si>
-  <si>
-    <t>uraeus@icloud.com</t>
-  </si>
-  <si>
-    <t>btech</t>
-  </si>
-  <si>
-    <t>cse</t>
-  </si>
-  <si>
-    <t>5th</t>
   </si>
 </sst>
 </file>
@@ -65,8 +49,10 @@
   <fonts count="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -89,17 +75,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -178,7 +161,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -213,7 +195,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -390,19 +371,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -430,55 +405,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>3568981</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="1"/>
-    </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>